<commit_message>
updated comp 220 with Sector and Class
</commit_message>
<xml_diff>
--- a/comp230/invoices.xlsx
+++ b/comp230/invoices.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gregf\OneDrive\Documents\EvolveU_BackEnd\comp230\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Greglaptop_old12/EvolveU_coding/BackEnd_X/comp230/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C460948-6C41-4E3A-9516-C024C0C78046}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947F25BC-ACF0-1940-8872-2520E1E4A43A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{82468A8D-9950-43B5-8B11-63209BEF58F9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="13180" xr2:uid="{82468A8D-9950-43B5-8B11-63209BEF58F9}"/>
   </bookViews>
   <sheets>
     <sheet name="customers" sheetId="1" r:id="rId1"/>
     <sheet name="products" sheetId="4" r:id="rId2"/>
     <sheet name="invoices" sheetId="2" r:id="rId3"/>
     <sheet name="line_items" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>driver</t>
   </si>
@@ -125,45 +124,6 @@
   </si>
   <si>
     <t>Test Guy 2</t>
-  </si>
-  <si>
-    <t>Marlo Hartung - Avanti</t>
-  </si>
-  <si>
-    <t>Dickson - Arcurve - full stack developer</t>
-  </si>
-  <si>
-    <t>Jason Lindemann - Arcurve - full stack developer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">questons: </t>
-  </si>
-  <si>
-    <t>continuous integration of deployment - how do you handle.?  Build automatically, test and deploy all in one.</t>
-  </si>
-  <si>
-    <t>deployment and builds</t>
-  </si>
-  <si>
-    <t>value proposition on product</t>
-  </si>
-  <si>
-    <t>Why are you changing careers?</t>
-  </si>
-  <si>
-    <t>What are you doing next on product</t>
-  </si>
-  <si>
-    <t>What are you learning that's new, etc.</t>
-  </si>
-  <si>
-    <t>Mindfuel - Brent, Erik, Dare</t>
-  </si>
-  <si>
-    <t>Carolina - Inumerix</t>
-  </si>
-  <si>
-    <t>Max - Skip the dishes</t>
   </si>
 </sst>
 </file>
@@ -534,17 +494,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BF115F-5AA8-4253-812E-4BA511FBAB40}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -552,7 +512,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>7</v>
       </c>
@@ -560,7 +520,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>8</v>
       </c>
@@ -568,7 +528,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>13</v>
       </c>
@@ -576,7 +536,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>14</v>
       </c>
@@ -584,7 +544,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>15</v>
       </c>
@@ -592,7 +552,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>16</v>
       </c>
@@ -600,7 +560,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>17</v>
       </c>
@@ -608,7 +568,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>18</v>
       </c>
@@ -616,7 +576,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>19</v>
       </c>
@@ -624,7 +584,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20</v>
       </c>
@@ -632,7 +592,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>21</v>
       </c>
@@ -640,7 +600,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>38</v>
       </c>
@@ -648,7 +608,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>39</v>
       </c>
@@ -656,7 +616,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>38</v>
       </c>
@@ -677,15 +637,15 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -699,7 +659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -713,7 +673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -727,7 +687,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -741,7 +701,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -755,7 +715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -769,7 +729,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -783,7 +743,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -811,14 +771,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -829,7 +789,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>50</v>
       </c>
@@ -840,7 +800,7 @@
         <v>43497</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>51</v>
       </c>
@@ -851,7 +811,7 @@
         <v>43498</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>52</v>
       </c>
@@ -862,7 +822,7 @@
         <v>43499</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>53</v>
       </c>
@@ -873,7 +833,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>54</v>
       </c>
@@ -884,7 +844,7 @@
         <v>43501</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>55</v>
       </c>
@@ -895,7 +855,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>56</v>
       </c>
@@ -906,7 +866,7 @@
         <v>43503</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>57</v>
       </c>
@@ -917,7 +877,7 @@
         <v>43504</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>58</v>
       </c>
@@ -928,7 +888,7 @@
         <v>43505</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>59</v>
       </c>
@@ -939,7 +899,7 @@
         <v>43506</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>60</v>
       </c>
@@ -950,7 +910,7 @@
         <v>43507</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>61</v>
       </c>
@@ -961,7 +921,7 @@
         <v>43508</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>62</v>
       </c>
@@ -972,7 +932,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>63</v>
       </c>
@@ -983,7 +943,7 @@
         <v>43510</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>64</v>
       </c>
@@ -994,7 +954,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>65</v>
       </c>
@@ -1005,7 +965,7 @@
         <v>43512</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>66</v>
       </c>
@@ -1016,7 +976,7 @@
         <v>43513</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>67</v>
       </c>
@@ -1027,7 +987,7 @@
         <v>43514</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>68</v>
       </c>
@@ -1038,7 +998,7 @@
         <v>43515</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>69</v>
       </c>
@@ -1049,7 +1009,7 @@
         <v>43516</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>70</v>
       </c>
@@ -1060,7 +1020,7 @@
         <v>43517</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>71</v>
       </c>
@@ -1071,7 +1031,7 @@
         <v>43518</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>72</v>
       </c>
@@ -1082,7 +1042,7 @@
         <v>43519</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>73</v>
       </c>
@@ -1093,7 +1053,7 @@
         <v>43520</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>74</v>
       </c>
@@ -1104,7 +1064,7 @@
         <v>43521</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>75</v>
       </c>
@@ -1115,7 +1075,7 @@
         <v>43522</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>76</v>
       </c>
@@ -1126,43 +1086,43 @@
         <v>43523</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C41" s="1"/>
     </row>
   </sheetData>
@@ -1178,17 +1138,17 @@
   <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1199,7 +1159,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>50</v>
       </c>
@@ -1210,7 +1170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>50</v>
       </c>
@@ -1221,7 +1181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>51</v>
       </c>
@@ -1232,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>51</v>
       </c>
@@ -1243,7 +1203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>52</v>
       </c>
@@ -1254,7 +1214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>52</v>
       </c>
@@ -1265,7 +1225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>53</v>
       </c>
@@ -1276,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>53</v>
       </c>
@@ -1287,7 +1247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>54</v>
       </c>
@@ -1298,7 +1258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>54</v>
       </c>
@@ -1309,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>55</v>
       </c>
@@ -1320,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>55</v>
       </c>
@@ -1331,7 +1291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>55</v>
       </c>
@@ -1342,7 +1302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>56</v>
       </c>
@@ -1353,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>56</v>
       </c>
@@ -1364,7 +1324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>56</v>
       </c>
@@ -1375,7 +1335,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>56</v>
       </c>
@@ -1386,7 +1346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>57</v>
       </c>
@@ -1397,7 +1357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>57</v>
       </c>
@@ -1408,7 +1368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>57</v>
       </c>
@@ -1419,7 +1379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>57</v>
       </c>
@@ -1430,7 +1390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>57</v>
       </c>
@@ -1441,7 +1401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>58</v>
       </c>
@@ -1452,7 +1412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>58</v>
       </c>
@@ -1463,7 +1423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>58</v>
       </c>
@@ -1474,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>58</v>
       </c>
@@ -1485,7 +1445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>58</v>
       </c>
@@ -1496,7 +1456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>59</v>
       </c>
@@ -1507,7 +1467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>59</v>
       </c>
@@ -1518,7 +1478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>60</v>
       </c>
@@ -1529,7 +1489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>61</v>
       </c>
@@ -1540,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>61</v>
       </c>
@@ -1551,7 +1511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>62</v>
       </c>
@@ -1562,7 +1522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>63</v>
       </c>
@@ -1573,7 +1533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>63</v>
       </c>
@@ -1584,7 +1544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>63</v>
       </c>
@@ -1595,7 +1555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>64</v>
       </c>
@@ -1606,7 +1566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>65</v>
       </c>
@@ -1617,7 +1577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>66</v>
       </c>
@@ -1628,7 +1588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>66</v>
       </c>
@@ -1639,7 +1599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>66</v>
       </c>
@@ -1650,7 +1610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>67</v>
       </c>
@@ -1661,7 +1621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>68</v>
       </c>
@@ -1672,7 +1632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>68</v>
       </c>
@@ -1683,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>69</v>
       </c>
@@ -1694,7 +1654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>69</v>
       </c>
@@ -1705,7 +1665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>70</v>
       </c>
@@ -1716,7 +1676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>70</v>
       </c>
@@ -1727,7 +1687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>71</v>
       </c>
@@ -1738,7 +1698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>71</v>
       </c>
@@ -1749,7 +1709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>71</v>
       </c>
@@ -1760,7 +1720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>72</v>
       </c>
@@ -1771,7 +1731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>72</v>
       </c>
@@ -1782,7 +1742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>72</v>
       </c>
@@ -1793,7 +1753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>73</v>
       </c>
@@ -1804,7 +1764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>73</v>
       </c>
@@ -1815,7 +1775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>73</v>
       </c>
@@ -1826,7 +1786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>74</v>
       </c>
@@ -1837,7 +1797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>74</v>
       </c>
@@ -1848,7 +1808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>75</v>
       </c>
@@ -1859,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>75</v>
       </c>
@@ -1870,7 +1830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>75</v>
       </c>
@@ -1881,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>75</v>
       </c>
@@ -1892,7 +1852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>76</v>
       </c>
@@ -1903,7 +1863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>76</v>
       </c>
@@ -1914,7 +1874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>76</v>
       </c>
@@ -1925,7 +1885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>76</v>
       </c>
@@ -1936,7 +1896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>76</v>
       </c>
@@ -1947,7 +1907,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>76</v>
       </c>
@@ -1962,84 +1922,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDB8DD1-56A5-498B-AA33-96D82488F32D}">
-  <dimension ref="A1:A15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>